<commit_message>
[ADD]: Example report SXCN
</commit_message>
<xml_diff>
--- a/src/assets/ExcelSample/BLHH_CSSXCN/1.xlsx
+++ b/src/assets/ExcelSample/BLHH_CSSXCN/1.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VNPTBPC\tuhla.bpc\Coding\SCT\industrial-and-commercial-facilities\src\assets\ExcelSample\BLHH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VNPTBPC\tuhla.bpc\Coding\SCT\industrial-and-commercial-facilities\src\assets\ExcelSample\BLHH_CSSXCN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Tháng 1" sheetId="1" r:id="rId1"/>
+    <sheet name="BLHH" sheetId="1" r:id="rId1"/>
+    <sheet name="SXCN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -78,6 +79,108 @@
   </si>
   <si>
     <t>Thực hiện so với cùng kỳ  năm trước</t>
+  </si>
+  <si>
+    <t>Chỉ số sản xuất công nghiệp (IIP) so với cùng kỳ theo giá so sánh năm 2010</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Công nghiệp khai khoáng</t>
+  </si>
+  <si>
+    <t>Công nghiệp chế biến, chế tạo</t>
+  </si>
+  <si>
+    <t>Sản xuất và phân phối điện, khí đốt, nước</t>
+  </si>
+  <si>
+    <t>Cung cấp nước, quản lý và xử lý rác thải, nước thải</t>
+  </si>
+  <si>
+    <t>Một số sản phẩm công nghiệp chủ yếu</t>
+  </si>
+  <si>
+    <t>Đá xây dựng khác</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Hạt điều nhân</t>
+  </si>
+  <si>
+    <t>Tấn</t>
+  </si>
+  <si>
+    <t>Vải dệt nổi vòng, vải sonin từ sợi nhân tạo</t>
+  </si>
+  <si>
+    <t>1000 m2</t>
+  </si>
+  <si>
+    <t>Dịch vụ in từ sợi và vải (gồm cả đồ để mặc)</t>
+  </si>
+  <si>
+    <t>Dịch vụ hoàn thiện sản phẩm dệt khác</t>
+  </si>
+  <si>
+    <t>Quần án các loại</t>
+  </si>
+  <si>
+    <t>999 cái</t>
+  </si>
+  <si>
+    <t>Giày, dép có đế hoặc mũ bằng da</t>
+  </si>
+  <si>
+    <t>1000 đôi</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất giày, dép</t>
+  </si>
+  <si>
+    <t>Gỗ cưa, xẻ các loại</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Ván ép từ gỗ và các vật liệu tương tự</t>
+  </si>
+  <si>
+    <t>Bao bì và túi bằng giấy nhăn và bìa nhăn</t>
+  </si>
+  <si>
+    <t>1000 chiếc</t>
+  </si>
+  <si>
+    <t>Các hợp chất từ cao su tổng hợp và cao su tự nhiên và các loại nhựa tự nhiên tương tự, ở dạng nguyên sinh hoặc tấm lỏ hoặc dải</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất tấm, phiến, ống và các mặt nghiêng bằng plastic</t>
+  </si>
+  <si>
+    <t>Xi măng Portland đen</t>
+  </si>
+  <si>
+    <t>Chì chưa gia công</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất bao bì bằng kim loại</t>
+  </si>
+  <si>
+    <t>tử, bàn, đồ nội thất bàng gỗ</t>
+  </si>
+  <si>
+    <t>Chiếc</t>
+  </si>
+  <si>
+    <t>Điện sản xuất</t>
+  </si>
+  <si>
+    <t>Triệu KWh</t>
   </si>
 </sst>
 </file>
@@ -165,7 +268,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -188,6 +291,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -473,12 +577,12 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="60.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
@@ -596,4 +700,513 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>165</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>166</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>167</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>168</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>169</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>170</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>171</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>172</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>173</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>174</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>175</v>
+      </c>
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>176</v>
+      </c>
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>177</v>
+      </c>
+      <c r="B14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>178</v>
+      </c>
+      <c r="B15" s="4">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>179</v>
+      </c>
+      <c r="B16" s="4">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>180</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>181</v>
+      </c>
+      <c r="B18" s="4">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>182</v>
+      </c>
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>183</v>
+      </c>
+      <c r="B20" s="4">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>184</v>
+      </c>
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>185</v>
+      </c>
+      <c r="B22" s="4">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>186</v>
+      </c>
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>187</v>
+      </c>
+      <c r="B24" s="4">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>188</v>
+      </c>
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dev new report (#129)
* 26/10/2021

Thay đổi cấu trúc new_model
Thêm chức năng tổng hợp dữ liệu

* 27/10/2021

Cập nhật lại tính năng tổng hợp dữ liệu

* [ADD]: Example report SXCN

Co-authored-by: toumeielegy <binhdo26.k42@st.ueh.edu.vn>
</commit_message>
<xml_diff>
--- a/src/assets/ExcelSample/BLHH_CSSXCN/1.xlsx
+++ b/src/assets/ExcelSample/BLHH_CSSXCN/1.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VNPTBPC\tuhla.bpc\Coding\SCT\industrial-and-commercial-facilities\src\assets\ExcelSample\BLHH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VNPTBPC\tuhla.bpc\Coding\SCT\industrial-and-commercial-facilities\src\assets\ExcelSample\BLHH_CSSXCN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Tháng 1" sheetId="1" r:id="rId1"/>
+    <sheet name="BLHH" sheetId="1" r:id="rId1"/>
+    <sheet name="SXCN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -78,6 +79,108 @@
   </si>
   <si>
     <t>Thực hiện so với cùng kỳ  năm trước</t>
+  </si>
+  <si>
+    <t>Chỉ số sản xuất công nghiệp (IIP) so với cùng kỳ theo giá so sánh năm 2010</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Công nghiệp khai khoáng</t>
+  </si>
+  <si>
+    <t>Công nghiệp chế biến, chế tạo</t>
+  </si>
+  <si>
+    <t>Sản xuất và phân phối điện, khí đốt, nước</t>
+  </si>
+  <si>
+    <t>Cung cấp nước, quản lý và xử lý rác thải, nước thải</t>
+  </si>
+  <si>
+    <t>Một số sản phẩm công nghiệp chủ yếu</t>
+  </si>
+  <si>
+    <t>Đá xây dựng khác</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Hạt điều nhân</t>
+  </si>
+  <si>
+    <t>Tấn</t>
+  </si>
+  <si>
+    <t>Vải dệt nổi vòng, vải sonin từ sợi nhân tạo</t>
+  </si>
+  <si>
+    <t>1000 m2</t>
+  </si>
+  <si>
+    <t>Dịch vụ in từ sợi và vải (gồm cả đồ để mặc)</t>
+  </si>
+  <si>
+    <t>Dịch vụ hoàn thiện sản phẩm dệt khác</t>
+  </si>
+  <si>
+    <t>Quần án các loại</t>
+  </si>
+  <si>
+    <t>999 cái</t>
+  </si>
+  <si>
+    <t>Giày, dép có đế hoặc mũ bằng da</t>
+  </si>
+  <si>
+    <t>1000 đôi</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất giày, dép</t>
+  </si>
+  <si>
+    <t>Gỗ cưa, xẻ các loại</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Ván ép từ gỗ và các vật liệu tương tự</t>
+  </si>
+  <si>
+    <t>Bao bì và túi bằng giấy nhăn và bìa nhăn</t>
+  </si>
+  <si>
+    <t>1000 chiếc</t>
+  </si>
+  <si>
+    <t>Các hợp chất từ cao su tổng hợp và cao su tự nhiên và các loại nhựa tự nhiên tương tự, ở dạng nguyên sinh hoặc tấm lỏ hoặc dải</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất tấm, phiến, ống và các mặt nghiêng bằng plastic</t>
+  </si>
+  <si>
+    <t>Xi măng Portland đen</t>
+  </si>
+  <si>
+    <t>Chì chưa gia công</t>
+  </si>
+  <si>
+    <t>Dịch vụ sản xuất bao bì bằng kim loại</t>
+  </si>
+  <si>
+    <t>tử, bàn, đồ nội thất bàng gỗ</t>
+  </si>
+  <si>
+    <t>Chiếc</t>
+  </si>
+  <si>
+    <t>Điện sản xuất</t>
+  </si>
+  <si>
+    <t>Triệu KWh</t>
   </si>
 </sst>
 </file>
@@ -165,7 +268,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -188,6 +291,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -473,12 +577,12 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="60.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
@@ -596,4 +700,513 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>165</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>166</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>167</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>168</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>169</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>170</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>171</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>172</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>173</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>174</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>175</v>
+      </c>
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>176</v>
+      </c>
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>177</v>
+      </c>
+      <c r="B14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>178</v>
+      </c>
+      <c r="B15" s="4">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>179</v>
+      </c>
+      <c r="B16" s="4">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>180</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>181</v>
+      </c>
+      <c r="B18" s="4">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>182</v>
+      </c>
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>183</v>
+      </c>
+      <c r="B20" s="4">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>184</v>
+      </c>
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>185</v>
+      </c>
+      <c r="B22" s="4">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>186</v>
+      </c>
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>187</v>
+      </c>
+      <c r="B24" s="4">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>188</v>
+      </c>
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>